<commit_message>
add restrict in register name(not more than 20)
</commit_message>
<xml_diff>
--- a/CourseList.xlsx
+++ b/CourseList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/Eclipse  WorkSpace/TrainingDepartment/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/thetnainglin/eclipse_workspace_old/TrainingDepartment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5A752C-B53E-254D-82AD-2D846B90B722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D52B89-7D0B-CC41-9046-0F316DA7FE79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4680" yWindow="3440" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4680" yWindow="4040" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="March_CourseList" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Adobe Photoshop (Morning) (30000ks)</t>
   </si>
@@ -49,7 +49,10 @@
     <t>Choose Your Course</t>
   </si>
   <si>
-    <t>CIA (morning)</t>
+    <t>CIA(Evening)</t>
+  </si>
+  <si>
+    <t>CIA (Morning)</t>
   </si>
 </sst>
 </file>
@@ -890,10 +893,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -948,6 +951,11 @@
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>